<commit_message>
base de dados consolidada
</commit_message>
<xml_diff>
--- a/data/DADOS CONSOLIDADOS.xlsx
+++ b/data/DADOS CONSOLIDADOS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Automation System\Chiquinho_dash\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126C143A-27A9-46A3-A8ED-230F93AB209E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B34FAA9-067C-4997-A4A4-E66DD674A462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C3B3B883-1BCA-427C-9F3D-3E207A053364}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="7" xr2:uid="{C3B3B883-1BCA-427C-9F3D-3E207A053364}"/>
   </bookViews>
   <sheets>
     <sheet name="REGISTRO DE CONTAS" sheetId="9" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5183" uniqueCount="1290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5212" uniqueCount="1299">
   <si>
     <t>TOTAL</t>
   </si>
@@ -3725,9 +3725,6 @@
     <t>despesas</t>
   </si>
   <si>
-    <t>PASSAGEM</t>
-  </si>
-  <si>
     <t>3031695</t>
   </si>
   <si>
@@ -3776,27 +3773,6 @@
     <t>Observação</t>
   </si>
   <si>
-    <t>Compra de leite</t>
-  </si>
-  <si>
-    <t>Insumo</t>
-  </si>
-  <si>
-    <t>Dinheiro próprio</t>
-  </si>
-  <si>
-    <t>Não registrado no caixa</t>
-  </si>
-  <si>
-    <t>Lanche funcionários</t>
-  </si>
-  <si>
-    <t>RH</t>
-  </si>
-  <si>
-    <t>Pix do gerente</t>
-  </si>
-  <si>
     <t>Faltas</t>
   </si>
   <si>
@@ -3915,6 +3891,57 @@
   </si>
   <si>
     <t>CONTA DE ÁGUA</t>
+  </si>
+  <si>
+    <t>PASSAGEM ELIEVERTON</t>
+  </si>
+  <si>
+    <t>PASSAGEM REUNIÃO -POLIANA</t>
+  </si>
+  <si>
+    <t>Cx leite líquido 1L</t>
+  </si>
+  <si>
+    <t>Insumos</t>
+  </si>
+  <si>
+    <t>Leite em pó Ninho</t>
+  </si>
+  <si>
+    <t>Tábua e Bom Ar</t>
+  </si>
+  <si>
+    <t>Materiais</t>
+  </si>
+  <si>
+    <t>Limão</t>
+  </si>
+  <si>
+    <t>Biscoito Maisena e açúcar</t>
+  </si>
+  <si>
+    <t>Morangos</t>
+  </si>
+  <si>
+    <t>Panificação (pão, massa, etc.)</t>
+  </si>
+  <si>
+    <t>Transporte</t>
+  </si>
+  <si>
+    <t>Transporte / Outros</t>
+  </si>
+  <si>
+    <t>Sabonete 5L antisséptico</t>
+  </si>
+  <si>
+    <t>Porta sabonete, reservatório, canetas e trincha</t>
+  </si>
+  <si>
+    <t>Reservatório</t>
+  </si>
+  <si>
+    <t>Passagem Mariana</t>
   </si>
 </sst>
 </file>
@@ -4254,9 +4281,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -4299,19 +4323,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4345,263 +4356,28 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="35">
-    <dxf>
-      <font>
-        <color rgb="FFFAE2D5"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF8989"/>
-          <bgColor rgb="FFFF8989"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFD9F2D0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00B050"/>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFCC"/>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF275317"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB3E5A1"/>
-          <bgColor rgb="FFB3E5A1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.79998168889431442"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF8989"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="0.79998168889431442"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFAE2D5"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF8989"/>
-          <bgColor rgb="FFFF8989"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFD9F2D0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00B050"/>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFCC"/>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF275317"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB3E5A1"/>
-          <bgColor rgb="FFB3E5A1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="27">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4679,6 +4455,50 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFAE2D5"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF8989"/>
+          <bgColor rgb="FFFF8989"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFD9F2D0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00B050"/>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFCC"/>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF275317"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB3E5A1"/>
+          <bgColor rgb="FFB3E5A1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4811,6 +4631,129 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -4897,21 +4840,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C0FE7D5F-0D9D-47E7-B50B-3C06D9E210A9}" name="Tabela2" displayName="Tabela2" ref="A3:J15" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" totalsRowBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C0FE7D5F-0D9D-47E7-B50B-3C06D9E210A9}" name="Tabela2" displayName="Tabela2" ref="A3:J15" totalsRowShown="0" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25" tableBorderDxfId="23" totalsRowBorderDxfId="22">
   <autoFilter ref="A3:J15" xr:uid="{606281A0-31C5-4F75-831E-D3B54F682EEC}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{E96BCBD6-7AAC-4BC4-B2E1-246296DFD938}" name="ID" dataDxfId="29"/>
-    <tableColumn id="12" xr3:uid="{659BDB55-9086-4F7A-8631-61B50EEAE3A6}" name="FORNECEDOR" dataDxfId="12"/>
-    <tableColumn id="11" xr3:uid="{E77F8A71-C06E-4B6E-8AF2-D93918C32869}" name="DESCRIÇÃO" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{DD35B5CA-5F65-4766-B8AC-D1A819CAE283}" name="VALOR" dataDxfId="10" dataCellStyle="Moeda"/>
-    <tableColumn id="3" xr3:uid="{5ACB18B0-BD83-4ECA-B2E7-ACE3966ED371}" name="DATA VENCIMENTO" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{7AF2AF21-C35E-4D74-A739-5EB71A734272}" name="STATUS" dataDxfId="8">
+    <tableColumn id="1" xr3:uid="{E96BCBD6-7AAC-4BC4-B2E1-246296DFD938}" name="ID" dataDxfId="21"/>
+    <tableColumn id="12" xr3:uid="{659BDB55-9086-4F7A-8631-61B50EEAE3A6}" name="FORNECEDOR" dataDxfId="20"/>
+    <tableColumn id="11" xr3:uid="{E77F8A71-C06E-4B6E-8AF2-D93918C32869}" name="DESCRIÇÃO" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{DD35B5CA-5F65-4766-B8AC-D1A819CAE283}" name="VALOR" dataDxfId="18" dataCellStyle="Moeda"/>
+    <tableColumn id="3" xr3:uid="{5ACB18B0-BD83-4ECA-B2E7-ACE3966ED371}" name="DATA VENCIMENTO" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{7AF2AF21-C35E-4D74-A739-5EB71A734272}" name="STATUS" dataDxfId="16">
       <calculatedColumnFormula>IF(J4="OK","PAGO",IF(E4-$D$1=0,"VENCE HOJE",IF(E4-$D$1&lt;0,"VENCIDO","A VENCER")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{BC0BD493-2DBC-42B5-AFA8-D4D8B3CB9265}" name="LINK BOLETO" dataDxfId="28"/>
-    <tableColumn id="8" xr3:uid="{CB84E09D-E8B4-4FCA-BDF0-D8E75A741D45}" name="DATA DE PAGAMENTO" dataDxfId="27"/>
-    <tableColumn id="9" xr3:uid="{6DCB057D-35FE-427C-9730-8E57BB5099AC}" name="FORMA DE PAGAMENTO" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{5D6DC5FE-109B-483C-B136-F6E57BD1C758}" name="PAGO" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{BC0BD493-2DBC-42B5-AFA8-D4D8B3CB9265}" name="LINK BOLETO" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{CB84E09D-E8B4-4FCA-BDF0-D8E75A741D45}" name="DATA DE PAGAMENTO" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{6DCB057D-35FE-427C-9730-8E57BB5099AC}" name="FORMA DE PAGAMENTO" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{5D6DC5FE-109B-483C-B136-F6E57BD1C758}" name="PAGO" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5236,7 +5179,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0078630-9221-4A13-898E-62F6FB7B8B87}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
@@ -5249,377 +5192,377 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
-        <v>1254</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="13">
+      <c r="A1" s="36" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B1" s="37"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="12">
         <f ca="1">TODAY()</f>
         <v>46000</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>1248</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>1249</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>1250</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>1251</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>1252</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>1253</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>1254</v>
+      </c>
+      <c r="I3" s="14" t="s">
         <v>1255</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="J3" s="14" t="s">
         <v>1256</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>1257</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>1258</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>1259</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>1260</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>1261</v>
-      </c>
-      <c r="H3" s="15" t="s">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="15">
+        <v>1</v>
+      </c>
+      <c r="B4" s="25" t="s">
         <v>1262</v>
       </c>
-      <c r="I3" s="15" t="s">
-        <v>1263</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>1264</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="16">
-        <v>1</v>
-      </c>
-      <c r="B4" s="31" t="s">
-        <v>1270</v>
-      </c>
-      <c r="C4" s="31" t="s">
-        <v>1279</v>
-      </c>
-      <c r="D4" s="32">
+      <c r="C4" s="25" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D4" s="26">
         <v>220.6</v>
       </c>
-      <c r="E4" s="33">
+      <c r="E4" s="27">
         <v>46372</v>
       </c>
-      <c r="F4" s="34" t="str">
+      <c r="F4" s="28" t="str">
         <f t="shared" ref="F4:F13" ca="1" si="0">IF(J4="OK","PAGO",IF(E4-$D$1=0,"VENCE HOJE",IF(E4-$D$1&lt;0,"VENCIDO","A VENCER")))</f>
         <v>A VENCER</v>
       </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="18"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="17"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="16">
+      <c r="A5" s="15">
         <v>2</v>
       </c>
-      <c r="B5" s="31" t="s">
-        <v>1271</v>
-      </c>
-      <c r="C5" s="31" t="s">
-        <v>1280</v>
-      </c>
-      <c r="D5" s="32">
+      <c r="B5" s="25" t="s">
+        <v>1263</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>1272</v>
+      </c>
+      <c r="D5" s="26">
         <v>124.52</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="27">
         <v>46007</v>
       </c>
-      <c r="F5" s="34" t="str">
+      <c r="F5" s="28" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>A VENCER</v>
       </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="18"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="17"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="16">
+      <c r="A6" s="15">
         <v>3</v>
       </c>
-      <c r="B6" s="31" t="s">
-        <v>1272</v>
-      </c>
-      <c r="C6" s="31" t="s">
-        <v>1281</v>
-      </c>
-      <c r="D6" s="32">
+      <c r="B6" s="25" t="s">
+        <v>1264</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>1273</v>
+      </c>
+      <c r="D6" s="26">
         <v>230.3</v>
       </c>
-      <c r="E6" s="33">
+      <c r="E6" s="27">
         <v>46008</v>
       </c>
-      <c r="F6" s="34" t="str">
+      <c r="F6" s="28" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>A VENCER</v>
       </c>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="18"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="17"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="16">
+      <c r="A7" s="15">
         <v>4</v>
       </c>
-      <c r="B7" s="31" t="s">
-        <v>1273</v>
-      </c>
-      <c r="C7" s="31" t="s">
-        <v>1282</v>
-      </c>
-      <c r="D7" s="32">
+      <c r="B7" s="25" t="s">
+        <v>1265</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>1274</v>
+      </c>
+      <c r="D7" s="26">
         <v>57</v>
       </c>
-      <c r="E7" s="33">
+      <c r="E7" s="27">
         <v>46010</v>
       </c>
-      <c r="F7" s="34" t="str">
+      <c r="F7" s="28" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>A VENCER</v>
       </c>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="21"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="20"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="16">
+      <c r="A8" s="15">
         <v>5</v>
       </c>
-      <c r="B8" s="31" t="s">
-        <v>1274</v>
-      </c>
-      <c r="C8" s="31" t="s">
-        <v>1283</v>
-      </c>
-      <c r="D8" s="32">
+      <c r="B8" s="25" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D8" s="26">
         <v>605.21</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8" s="27">
         <v>46009</v>
       </c>
-      <c r="F8" s="34" t="str">
+      <c r="F8" s="28" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>A VENCER</v>
       </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="18"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="17"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="16">
+      <c r="A9" s="15">
         <v>6</v>
       </c>
-      <c r="B9" s="31" t="s">
-        <v>1275</v>
-      </c>
-      <c r="C9" s="31" t="s">
-        <v>1284</v>
-      </c>
-      <c r="D9" s="32">
+      <c r="B9" s="25" t="s">
+        <v>1267</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>1276</v>
+      </c>
+      <c r="D9" s="26">
         <v>6062.7</v>
       </c>
-      <c r="E9" s="33">
+      <c r="E9" s="27">
         <v>46008</v>
       </c>
-      <c r="F9" s="34" t="str">
+      <c r="F9" s="28" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>A VENCER</v>
       </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="18"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="17"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="16">
+      <c r="A10" s="15">
         <v>7</v>
       </c>
-      <c r="B10" s="31" t="s">
-        <v>1275</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>1285</v>
-      </c>
-      <c r="D10" s="32">
+      <c r="B10" s="25" t="s">
+        <v>1267</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>1277</v>
+      </c>
+      <c r="D10" s="26">
         <v>6062.7</v>
       </c>
-      <c r="E10" s="33">
+      <c r="E10" s="27">
         <v>46015</v>
       </c>
-      <c r="F10" s="34" t="str">
+      <c r="F10" s="28" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>A VENCER</v>
       </c>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="18"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="17"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="16">
+      <c r="A11" s="15">
         <v>8</v>
       </c>
-      <c r="B11" s="31" t="s">
-        <v>1276</v>
-      </c>
-      <c r="C11" s="35" t="s">
-        <v>1286</v>
-      </c>
-      <c r="D11" s="32">
+      <c r="B11" s="25" t="s">
+        <v>1268</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>1278</v>
+      </c>
+      <c r="D11" s="26">
         <v>1263.71</v>
       </c>
-      <c r="E11" s="33">
+      <c r="E11" s="27">
         <v>46013</v>
       </c>
-      <c r="F11" s="34" t="str">
+      <c r="F11" s="28" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>A VENCER</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="18"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="17"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="16">
+      <c r="A12" s="15">
         <v>9</v>
       </c>
-      <c r="B12" s="31" t="s">
-        <v>1276</v>
-      </c>
-      <c r="C12" s="35" t="s">
-        <v>1286</v>
-      </c>
-      <c r="D12" s="32">
+      <c r="B12" s="25" t="s">
+        <v>1268</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>1278</v>
+      </c>
+      <c r="D12" s="26">
         <v>1263.71</v>
       </c>
-      <c r="E12" s="33">
+      <c r="E12" s="27">
         <v>46021</v>
       </c>
-      <c r="F12" s="34" t="str">
+      <c r="F12" s="28" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>A VENCER</v>
       </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="18"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="17"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="16">
+      <c r="A13" s="15">
         <v>10</v>
       </c>
-      <c r="B13" s="31" t="s">
-        <v>1277</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>1287</v>
-      </c>
-      <c r="D13" s="32">
+      <c r="B13" s="25" t="s">
+        <v>1269</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>1279</v>
+      </c>
+      <c r="D13" s="26">
         <v>2672.6</v>
       </c>
-      <c r="E13" s="33">
+      <c r="E13" s="27">
         <v>46020</v>
       </c>
-      <c r="F13" s="34" t="str">
+      <c r="F13" s="28" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>A VENCER</v>
       </c>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="18"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="17"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="16">
+      <c r="A14" s="15">
         <v>11</v>
       </c>
-      <c r="B14" s="31" t="s">
-        <v>1278</v>
-      </c>
-      <c r="C14" s="31" t="s">
-        <v>1288</v>
-      </c>
-      <c r="D14" s="36">
+      <c r="B14" s="25" t="s">
+        <v>1270</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D14" s="30">
         <v>1461.13</v>
       </c>
-      <c r="E14" s="33">
+      <c r="E14" s="27">
         <v>45994</v>
       </c>
-      <c r="F14" s="37" t="str">
+      <c r="F14" s="31" t="str">
         <f t="shared" ref="F14:F15" ca="1" si="1">IF(J14="OK","PAGO",IF(E14-$D$1=0,"VENCE HOJE",IF(E14-$D$1&lt;0,"VENCIDO","A VENCER")))</f>
         <v>VENCIDO</v>
       </c>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="18"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="17"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="19">
+      <c r="A15" s="18">
         <v>12</v>
       </c>
-      <c r="B15" s="38" t="s">
-        <v>1269</v>
-      </c>
-      <c r="C15" s="38" t="s">
-        <v>1289</v>
-      </c>
-      <c r="D15" s="39">
+      <c r="B15" s="32" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>1281</v>
+      </c>
+      <c r="D15" s="33">
         <v>525.79999999999995</v>
       </c>
-      <c r="E15" s="40">
+      <c r="E15" s="34">
         <v>45994</v>
       </c>
-      <c r="F15" s="41" t="str">
+      <c r="F15" s="35" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>VENCIDO</v>
       </c>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="21"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
-  <conditionalFormatting sqref="G4:I15">
-    <cfRule type="cellIs" dxfId="24" priority="5" operator="equal">
+  <conditionalFormatting sqref="F4:F15">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"A VENCER"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"VENCE HOJE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>"PAGO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>"VENCIDO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4:F15">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
+  <conditionalFormatting sqref="G4:I15">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"A VENCER"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"VENCE HOJE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>"PAGO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
       <formula>"VENCIDO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5646,42 +5589,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>1252</v>
+        <v>1244</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>1253</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B2" t="s">
         <v>1231</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1232</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B3" t="s">
         <v>1233</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1234</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B4" t="s">
         <v>1235</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1236</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="B5" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
     </row>
   </sheetData>
@@ -5704,61 +5647,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="25.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
-        <v>1260</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>1265</v>
+      <c r="A1" s="21" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>1257</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="25.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
-        <v>1266</v>
-      </c>
-      <c r="B2" s="24">
+      <c r="A2" s="22" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B2" s="23">
         <f ca="1">SUMIF('REGISTRO DE CONTAS'!F:F,'RESUMO GERAL'!A2,'REGISTRO DE CONTAS'!D:D)</f>
         <v>18563.049999999996</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="25.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
-        <v>1267</v>
-      </c>
-      <c r="B3" s="24">
+      <c r="A3" s="24" t="s">
+        <v>1259</v>
+      </c>
+      <c r="B3" s="23">
         <f ca="1">SUMIF('REGISTRO DE CONTAS'!F:F,'RESUMO GERAL'!A3,'REGISTRO DE CONTAS'!D:D)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="25.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
-        <v>1268</v>
-      </c>
-      <c r="B4" s="24">
+      <c r="A4" s="22" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B4" s="23">
         <f ca="1">SUMIF('REGISTRO DE CONTAS'!F:F,'RESUMO GERAL'!A4,'REGISTRO DE CONTAS'!D:D)</f>
         <v>1986.93</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="25.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="25" t="s">
-        <v>1264</v>
-      </c>
-      <c r="B5" s="24">
+      <c r="A5" s="24" t="s">
+        <v>1256</v>
+      </c>
+      <c r="B5" s="23">
         <f ca="1">SUMIF('REGISTRO DE CONTAS'!F:F,'RESUMO GERAL'!A5,'REGISTRO DE CONTAS'!D:D)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A5">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"A VENCER"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"VENCE HOJE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"PAGO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"VENCIDO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22790,7 +22733,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22799,7 +22742,7 @@
     <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -22837,7 +22780,7 @@
         <v>1225</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1226</v>
+        <v>1283</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>72</v>
@@ -22845,7 +22788,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>1224</v>
@@ -22857,15 +22800,15 @@
         <v>1225</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>1227</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>1228</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>1229</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>1224</v>
@@ -22876,21 +22819,19 @@
       <c r="D4" s="3" t="s">
         <v>1225</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>1282</v>
+      </c>
       <c r="F4" s="3" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="7">
-        <v>150</v>
-      </c>
+      <c r="A6" s="39"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -22902,17 +22843,17 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{627F52E4-7611-47C4-B291-6A9705612481}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.109375" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" customWidth="1"/>
+    <col min="2" max="2" width="39.21875" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="17.5546875" customWidth="1"/>
     <col min="5" max="5" width="19.44140625" customWidth="1"/>
     <col min="6" max="6" width="22.88671875" customWidth="1"/>
@@ -22923,56 +22864,223 @@
         <v>1</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>1238</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>1239</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>1240</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>1241</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>1242</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="11">
-        <v>45996</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>1243</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>1244</v>
-      </c>
-      <c r="D2" s="12">
-        <v>32</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>1245</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>1246</v>
+        <v>45992</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>1284</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>1285</v>
+      </c>
+      <c r="D2" s="41">
+        <v>57.87</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
-        <v>45997</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>1247</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>1248</v>
-      </c>
-      <c r="D3" s="12">
+        <v>45996</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>1286</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>1285</v>
+      </c>
+      <c r="D3" s="41">
+        <v>61.97</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="11">
+        <v>45996</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>1287</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>1288</v>
+      </c>
+      <c r="D4" s="41">
         <v>45</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>1249</v>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="11">
+        <v>45993</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>1289</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>1285</v>
+      </c>
+      <c r="D5" s="41">
+        <v>9.84</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="11">
+        <v>45992</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>1290</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>1285</v>
+      </c>
+      <c r="D6" s="41">
+        <v>15.6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="11">
+        <v>45993</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>1291</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>1285</v>
+      </c>
+      <c r="D7" s="41">
+        <v>22.98</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="11">
+        <v>45993</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>1292</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>1285</v>
+      </c>
+      <c r="D8" s="41">
+        <v>21.83</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="11">
+        <v>45993</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>1293</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>1294</v>
+      </c>
+      <c r="D9" s="41">
+        <v>30.27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="11">
+        <v>45995</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>1295</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>1288</v>
+      </c>
+      <c r="D10" s="41">
+        <v>55</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="11">
+        <v>45996</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>1296</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>1288</v>
+      </c>
+      <c r="D11" s="41">
+        <v>45</v>
+      </c>
+      <c r="E11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="11">
+        <v>45996</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>1297</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>1288</v>
+      </c>
+      <c r="D12" s="41">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="11">
+        <v>45995</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>1293</v>
+      </c>
+      <c r="D13" s="41">
+        <v>45</v>
+      </c>
+      <c r="E13" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -22998,10 +23106,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>1250</v>
+        <v>1242</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>1251</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>